<commit_message>
Wix Export format changed
</commit_message>
<xml_diff>
--- a/sql/match.xlsx
+++ b/sql/match.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I31759\source\repos\BOSMAJ24\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697CFDA8-A9B8-4A3D-912B-DF89F0425800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E9887A-740E-4609-AA22-EC4DFCC5C0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{179502E4-8792-4238-80B4-7832BD261A10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t>J</t>
   </si>
@@ -89,196 +89,196 @@
     <t>Adam Foulston</t>
   </si>
   <si>
-    <t>Sofia Smith-Londoño</t>
+    <t>Eleanor Jane Tress</t>
+  </si>
+  <si>
+    <t>Silvia Di Stasio</t>
+  </si>
+  <si>
+    <t>Eliska Prokesova</t>
+  </si>
+  <si>
+    <t>Heung Kwan Hui</t>
+  </si>
+  <si>
+    <t>Ámer khudari</t>
+  </si>
+  <si>
+    <t>Oluwademilade Oduwole</t>
+  </si>
+  <si>
+    <t>Emmanuel Ekpiken</t>
+  </si>
+  <si>
+    <t>Ashleigh Carey</t>
+  </si>
+  <si>
+    <t>Javier Aquilar Martin</t>
+  </si>
+  <si>
+    <t>Laura Perez</t>
+  </si>
+  <si>
+    <t>Sirran Elves</t>
+  </si>
+  <si>
+    <t>Olga Baikova</t>
+  </si>
+  <si>
+    <t>Thalia Padilla</t>
+  </si>
+  <si>
+    <t>Pedro Brinceño Salazar</t>
+  </si>
+  <si>
+    <t>Debora Lima</t>
+  </si>
+  <si>
+    <t>Beatrice Muzi</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Alberto Fernandez Vadillo</t>
+  </si>
+  <si>
+    <t>Jolie Saulite</t>
+  </si>
+  <si>
+    <t>Angel Peinado</t>
+  </si>
+  <si>
+    <t>Leandro Charanga</t>
+  </si>
+  <si>
+    <t>Andre L Maingot</t>
+  </si>
+  <si>
+    <t>Bishwas Hamal</t>
+  </si>
+  <si>
+    <t>Beth Miriam</t>
+  </si>
+  <si>
+    <t>Camy Marina</t>
+  </si>
+  <si>
+    <t>Pebbles</t>
+  </si>
+  <si>
+    <t>Carlos Paz</t>
+  </si>
+  <si>
+    <t>Oriana</t>
+  </si>
+  <si>
+    <t>Dani K</t>
+  </si>
+  <si>
+    <t>Elijah Tella</t>
+  </si>
+  <si>
+    <t>Daniel Carbonero</t>
+  </si>
+  <si>
+    <t>Ayesha Chan</t>
+  </si>
+  <si>
+    <t>Daniel Chong</t>
+  </si>
+  <si>
+    <t>Gabriel Bravo Rivera</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Ola</t>
+  </si>
+  <si>
+    <t>Diego Garcia</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Giovana Brandi</t>
+  </si>
+  <si>
+    <t>Rafael Nardon</t>
+  </si>
+  <si>
+    <t>Jessica Kasfiki</t>
+  </si>
+  <si>
+    <t>Leon Walber</t>
+  </si>
+  <si>
+    <t>Katerina Sergeeva</t>
+  </si>
+  <si>
+    <t>Laura Ann Williams</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Carla</t>
+  </si>
+  <si>
+    <t>Marky Marc</t>
+  </si>
+  <si>
+    <t>Trevor Anthony</t>
+  </si>
+  <si>
+    <t>Ramiro Zapata</t>
+  </si>
+  <si>
+    <t>Mihaela</t>
+  </si>
+  <si>
+    <t>Rola</t>
+  </si>
+  <si>
+    <t>Stephanie Lucero</t>
+  </si>
+  <si>
+    <t>Flame Luconi</t>
+  </si>
+  <si>
+    <t>Pierre Henry</t>
+  </si>
+  <si>
+    <t>Ariana</t>
+  </si>
+  <si>
+    <t>James re</t>
+  </si>
+  <si>
+    <t>Christopher Webster</t>
+  </si>
+  <si>
+    <t>Su Jin Han</t>
+  </si>
+  <si>
+    <t>Bryan Wong</t>
+  </si>
+  <si>
+    <t>Gabor Takacs</t>
   </si>
   <si>
     <t>Irene Salva Lopez</t>
   </si>
   <si>
-    <t>Eleanor Jane Tress</t>
-  </si>
-  <si>
-    <t>Silvia Di Stasio</t>
-  </si>
-  <si>
-    <t>Eliska Prokesova</t>
-  </si>
-  <si>
-    <t>Heung Kwan Hui</t>
-  </si>
-  <si>
-    <t>Ámer khudari</t>
-  </si>
-  <si>
-    <t>Oluwademilade Oduwole</t>
-  </si>
-  <si>
-    <t>Emmanuel Ekpiken</t>
-  </si>
-  <si>
-    <t>Ashleigh Carey</t>
-  </si>
-  <si>
-    <t>Javier Aquilar Martin</t>
-  </si>
-  <si>
-    <t>Laura Perez</t>
-  </si>
-  <si>
-    <t>Sirran Elves</t>
-  </si>
-  <si>
-    <t>Olga Baikova</t>
-  </si>
-  <si>
-    <t>Thalia Padilla</t>
-  </si>
-  <si>
-    <t>Pedro Brinceño Salazar</t>
-  </si>
-  <si>
-    <t>Debora Lima</t>
-  </si>
-  <si>
-    <t>Beatrice Muzi</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Alberto Fernandez Vadillo</t>
-  </si>
-  <si>
-    <t>Jolie Saulite</t>
-  </si>
-  <si>
-    <t>Angel Peinado</t>
-  </si>
-  <si>
-    <t>Leandro Charanga</t>
-  </si>
-  <si>
-    <t>Andre L Maingot</t>
-  </si>
-  <si>
-    <t>Bishwas Hamal</t>
-  </si>
-  <si>
-    <t>Beth Miriam</t>
-  </si>
-  <si>
-    <t>Camy Marina</t>
-  </si>
-  <si>
-    <t>Pebbles</t>
-  </si>
-  <si>
-    <t>Carlos Paz</t>
-  </si>
-  <si>
-    <t>Oriana</t>
-  </si>
-  <si>
-    <t>Dani K</t>
-  </si>
-  <si>
-    <t>Elijah Tella</t>
-  </si>
-  <si>
-    <t>Daniel Carbonero</t>
-  </si>
-  <si>
-    <t>Ayesha Chan</t>
-  </si>
-  <si>
-    <t>Daniel Chong</t>
-  </si>
-  <si>
-    <t>Gabriel Bravo Rivera</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Diego</t>
-  </si>
-  <si>
-    <t>Ola</t>
-  </si>
-  <si>
-    <t>Diego Garcia</t>
-  </si>
-  <si>
-    <t>Patricia</t>
-  </si>
-  <si>
-    <t>Giovana Brandi</t>
-  </si>
-  <si>
-    <t>Rafael Nardon</t>
-  </si>
-  <si>
-    <t>Jessica Kasfiki</t>
-  </si>
-  <si>
-    <t>Leon Walber</t>
-  </si>
-  <si>
-    <t>Katerina Sergeeva</t>
-  </si>
-  <si>
-    <t>Laura Ann Williams</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>Leo</t>
-  </si>
-  <si>
-    <t>Carla</t>
-  </si>
-  <si>
-    <t>Marky Marc</t>
-  </si>
-  <si>
-    <t>Trevor Anthony</t>
-  </si>
-  <si>
-    <t>Ramiro Zapata</t>
-  </si>
-  <si>
-    <t>Mihaela</t>
-  </si>
-  <si>
-    <t>Rola</t>
-  </si>
-  <si>
-    <t>Stephanie Lucero</t>
-  </si>
-  <si>
-    <t>Flame Luconi</t>
-  </si>
-  <si>
-    <t>Pierre Henry</t>
-  </si>
-  <si>
-    <t>Ariana</t>
-  </si>
-  <si>
-    <t>James re</t>
-  </si>
-  <si>
-    <t>Christopher Webster</t>
-  </si>
-  <si>
-    <t>Oi Yean Wong</t>
-  </si>
-  <si>
-    <t>Su Jin Han</t>
-  </si>
-  <si>
-    <t>Bryan Wong</t>
+    <t>Sam Spencer</t>
   </si>
 </sst>
 </file>
@@ -353,8 +353,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{192C214A-26BB-4E3D-9E97-98BE52C1D6FE}" name="Table1" displayName="Table1" ref="A1:E42" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:E42" xr:uid="{192C214A-26BB-4E3D-9E97-98BE52C1D6FE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{192C214A-26BB-4E3D-9E97-98BE52C1D6FE}" name="Table1" displayName="Table1" ref="A1:E41" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:E41" xr:uid="{192C214A-26BB-4E3D-9E97-98BE52C1D6FE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E40">
+    <sortCondition ref="A2:A40"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4F286D0B-9B56-4DEE-B370-0BB8893FEA64}" name="Guest1"/>
     <tableColumn id="2" xr3:uid="{B78729A2-8D55-4557-AD5E-0256586F2C0C}" name="Guest2"/>
@@ -683,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E5A6B0-C99C-495A-B2DC-FB8D9439EA05}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -712,15 +715,15 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -734,10 +737,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -754,7 +757,7 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -768,7 +771,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -777,35 +783,32 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
@@ -816,10 +819,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
@@ -833,10 +836,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>2</v>
@@ -850,10 +853,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>2</v>
@@ -884,10 +887,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -896,15 +899,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
@@ -918,16 +921,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -935,16 +938,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -952,10 +955,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>2</v>
@@ -969,10 +972,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>2</v>
@@ -986,10 +989,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>2</v>
@@ -998,15 +1001,15 @@
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>2</v>
@@ -1020,10 +1023,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>2</v>
@@ -1037,126 +1040,129 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1164,24 +1170,27 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
@@ -1195,10 +1204,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
@@ -1207,21 +1216,18 @@
         <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -1229,30 +1235,33 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -1260,27 +1269,21 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>2</v>
@@ -1289,15 +1292,15 @@
         <v>1</v>
       </c>
       <c r="E36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>2</v>
@@ -1311,10 +1314,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>2</v>
@@ -1323,12 +1326,12 @@
         <v>1</v>
       </c>
       <c r="E38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>2</v>
@@ -1342,7 +1345,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>2</v>
@@ -1351,21 +1357,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>